<commit_message>
implemented mixed models (master/guesser)
</commit_message>
<xml_diff>
--- a/experiment_data/cot_data/cot_data_2.xlsx
+++ b/experiment_data/cot_data/cot_data_2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>red_cot</t>
   </si>
@@ -1306,6 +1306,36 @@
       <c r="B24" t="b">
         <v>0</v>
       </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="G24">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="b">
@@ -1313,6 +1343,36 @@
       </c>
       <c r="B25" t="b">
         <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>2.25</v>
+      </c>
+      <c r="E25">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12">

</xml_diff>